<commit_message>
Commit with working graphs in jupyter
</commit_message>
<xml_diff>
--- a/ice_cream_store/ice_cream_trends/report_data/Temperature.xlsx
+++ b/ice_cream_store/ice_cream_trends/report_data/Temperature.xlsx
@@ -348,63 +348,63 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
-        <v>17.85714285714286</v>
+        <v>19</v>
       </c>
       <c r="B1">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>17.42857142857143</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>14.42857142857143</v>
+        <v>16</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>6.571428571428571</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>15.71428571428571</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>12.71428571428571</v>
+        <v>20</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B7">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>15</v>
@@ -412,343 +412,343 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>24.42857142857143</v>
+        <v>22</v>
       </c>
       <c r="B10">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>23.71428571428572</v>
+        <v>26</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>13.57142857142857</v>
+        <v>21</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>23.28571428571428</v>
+        <v>18</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>12.57142857142857</v>
+        <v>21</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>24.85714285714286</v>
+        <v>22</v>
       </c>
       <c r="B17">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>17.28571428571428</v>
+        <v>13</v>
       </c>
       <c r="B18">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>17.14285714285714</v>
+        <v>22</v>
       </c>
       <c r="B19">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>20.85714285714286</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>11.71428571428571</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>17.28571428571428</v>
+        <v>15</v>
       </c>
       <c r="B23">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>10.71428571428571</v>
+        <v>18</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>15.14285714285714</v>
+        <v>16</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>17.14285714285714</v>
+        <v>21</v>
       </c>
       <c r="B26">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>25.71428571428572</v>
+        <v>17</v>
       </c>
       <c r="B27">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>16.42857142857143</v>
+        <v>17</v>
       </c>
       <c r="B28">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>15.28571428571429</v>
+        <v>20</v>
       </c>
       <c r="B29">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>15.85714285714286</v>
+        <v>14</v>
       </c>
       <c r="B30">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>22.28571428571428</v>
+        <v>21</v>
       </c>
       <c r="B31">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>20.28571428571428</v>
+        <v>24</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>22.42857142857143</v>
+        <v>21</v>
       </c>
       <c r="B34">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>21.85714285714286</v>
+        <v>26</v>
       </c>
       <c r="B35">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>13.14285714285714</v>
+        <v>22</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>22.14285714285714</v>
+        <v>14</v>
       </c>
       <c r="B37">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>24.28571428571428</v>
+        <v>20</v>
       </c>
       <c r="B38">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>25.42857142857143</v>
+        <v>19</v>
       </c>
       <c r="B39">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>25.14285714285714</v>
+        <v>20</v>
       </c>
       <c r="B40">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>20.57142857142857</v>
+        <v>18</v>
       </c>
       <c r="B41">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>15.71428571428571</v>
+        <v>9</v>
       </c>
       <c r="B42">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>11.85714285714286</v>
+        <v>15</v>
       </c>
       <c r="B43">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>19.14285714285714</v>
+        <v>17</v>
       </c>
       <c r="B44">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>18.57142857142857</v>
+        <v>13</v>
       </c>
       <c r="B45">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>13.85714285714286</v>
+        <v>24</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>15.85714285714286</v>
+        <v>16</v>
       </c>
       <c r="B47">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>23.71428571428572</v>
+        <v>21</v>
       </c>
       <c r="B48">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>19.57142857142857</v>
+        <v>19</v>
       </c>
       <c r="B49">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>21.71428571428572</v>
+        <v>13</v>
       </c>
       <c r="B50">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>20.14285714285714</v>
+        <v>21</v>
       </c>
       <c r="B51">
         <v>20</v>
@@ -756,10 +756,10 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B52">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>